<commit_message>
Continued 3.0 in Project Plan Lachlan doc
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/lachlan_dietrich_griffithuni_edu_au/Documents/Uni/2810ICT/Assignment 1 Part A/2810ICT-Assignment-1-Part-A/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_E0C8A7F0515C29AAE5B1393562E56DCE2A14542E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63FA087A-1D21-4B1E-9836-EC9368583E17}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -263,7 +264,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -300,17 +301,20 @@
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="7"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -551,7 +555,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,7 +586,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -618,83 +622,74 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -826,128 +821,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1189,28 +1062,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="7" max="7" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="43" max="52" width="3.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
@@ -1253,33 +1127,33 @@
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
+      <c r="AI2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
@@ -1937,79 +1811,83 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H5:BO39">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="12">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter differentFirst="1">
-    <oddFooter>Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
+  <headerFooter differentFirst="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Gantt Chart Updated as per the project
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F6DF6F2-C940-429B-B1A6-6BCE8ADDA190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -248,13 +247,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
-    <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="168" formatCode="d"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -609,7 +608,7 @@
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -618,10 +617,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" applyFill="0">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyFill="0">
@@ -655,13 +654,13 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,7 +678,7 @@
     <xf numFmtId="9" fontId="4" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,10 +690,10 @@
     <xf numFmtId="9" fontId="4" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -706,10 +705,10 @@
     <xf numFmtId="9" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,10 +720,10 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -783,7 +782,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="7">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="10">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="10">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="12">
@@ -800,18 +799,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -819,23 +806,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="20" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
+    <cellStyle name="Name" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Project Start" xfId="9"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -963,7 +962,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="11"/>
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="totalRow" dxfId="9"/>
@@ -1086,7 +1085,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1383,31 +1382,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BK29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="48" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="8" max="63" width="2.5703125" customWidth="1"/>
-    <col min="68" max="69" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="63" width="2.5546875" customWidth="1"/>
+    <col min="68" max="69" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="49" t="s">
         <v>28</v>
       </c>
@@ -1420,7 +1419,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="56"/>
     </row>
-    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>24</v>
       </c>
@@ -1429,19 +1428,18 @@
       </c>
       <c r="H2" s="57"/>
     </row>
-    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="59"/>
-      <c r="D3" s="63">
-        <f>DATEVALUE("14/08/2023")</f>
-        <v>45152</v>
-      </c>
-      <c r="E3" s="63"/>
-    </row>
-    <row r="4" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="66">
+        <v>45159</v>
+      </c>
+      <c r="E3" s="66"/>
+    </row>
+    <row r="4" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>29</v>
       </c>
@@ -1449,88 +1447,88 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="60">
+      <c r="H4" s="63">
         <f>H5</f>
-        <v>45152</v>
-      </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="60">
+        <v>45159</v>
+      </c>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="63">
         <f>O5</f>
-        <v>45159</v>
-      </c>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="60">
+        <v>45166</v>
+      </c>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="63">
         <f>V5</f>
-        <v>45166</v>
-      </c>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="60">
+        <v>45173</v>
+      </c>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="63">
         <f>AC5</f>
-        <v>45173</v>
-      </c>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="61"/>
-      <c r="AF4" s="61"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="62"/>
-      <c r="AJ4" s="60">
+        <v>45180</v>
+      </c>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="65"/>
+      <c r="AJ4" s="63">
         <f>AJ5</f>
-        <v>45180</v>
-      </c>
-      <c r="AK4" s="61"/>
-      <c r="AL4" s="61"/>
-      <c r="AM4" s="61"/>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="61"/>
-      <c r="AP4" s="62"/>
-      <c r="AQ4" s="60">
+        <v>45187</v>
+      </c>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="64"/>
+      <c r="AO4" s="64"/>
+      <c r="AP4" s="65"/>
+      <c r="AQ4" s="63">
         <f>AQ5</f>
-        <v>45187</v>
-      </c>
-      <c r="AR4" s="61"/>
-      <c r="AS4" s="61"/>
-      <c r="AT4" s="61"/>
-      <c r="AU4" s="61"/>
-      <c r="AV4" s="61"/>
-      <c r="AW4" s="62"/>
-      <c r="AX4" s="60">
+        <v>45194</v>
+      </c>
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="64"/>
+      <c r="AT4" s="64"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="65"/>
+      <c r="AX4" s="63">
         <f>AX5</f>
-        <v>45194</v>
-      </c>
-      <c r="AY4" s="61"/>
-      <c r="AZ4" s="61"/>
-      <c r="BA4" s="61"/>
-      <c r="BB4" s="61"/>
-      <c r="BC4" s="61"/>
-      <c r="BD4" s="62"/>
-      <c r="BE4" s="60">
+        <v>45201</v>
+      </c>
+      <c r="AY4" s="64"/>
+      <c r="AZ4" s="64"/>
+      <c r="BA4" s="64"/>
+      <c r="BB4" s="64"/>
+      <c r="BC4" s="64"/>
+      <c r="BD4" s="65"/>
+      <c r="BE4" s="63">
         <f>BE5</f>
-        <v>45201</v>
-      </c>
-      <c r="BF4" s="61"/>
-      <c r="BG4" s="61"/>
-      <c r="BH4" s="61"/>
-      <c r="BI4" s="61"/>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="62"/>
-    </row>
-    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45208</v>
+      </c>
+      <c r="BF4" s="64"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="64"/>
+      <c r="BJ4" s="64"/>
+      <c r="BK4" s="65"/>
+    </row>
+    <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>30</v>
       </c>
@@ -1541,230 +1539,230 @@
       <c r="F5" s="55"/>
       <c r="H5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45152</v>
+        <v>45159</v>
       </c>
       <c r="I5" s="9">
         <f>H5+1</f>
-        <v>45153</v>
+        <v>45160</v>
       </c>
       <c r="J5" s="9">
         <f>I5+1</f>
-        <v>45154</v>
+        <v>45161</v>
       </c>
       <c r="K5" s="9">
-        <f t="shared" ref="J5:AW5" si="0">J5+1</f>
-        <v>45155</v>
+        <f t="shared" ref="K5:AW5" si="0">J5+1</f>
+        <v>45162</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="0"/>
-        <v>45156</v>
+        <v>45163</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" si="0"/>
-        <v>45157</v>
+        <v>45164</v>
       </c>
       <c r="N5" s="11">
         <f t="shared" si="0"/>
-        <v>45158</v>
+        <v>45165</v>
       </c>
       <c r="O5" s="10">
         <f>N5+1</f>
-        <v>45159</v>
+        <v>45166</v>
       </c>
       <c r="P5" s="9">
         <f>O5+1</f>
-        <v>45160</v>
+        <v>45167</v>
       </c>
       <c r="Q5" s="9">
         <f t="shared" si="0"/>
-        <v>45161</v>
+        <v>45168</v>
       </c>
       <c r="R5" s="9">
         <f t="shared" si="0"/>
-        <v>45162</v>
+        <v>45169</v>
       </c>
       <c r="S5" s="9">
         <f t="shared" si="0"/>
-        <v>45163</v>
+        <v>45170</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" si="0"/>
-        <v>45164</v>
+        <v>45171</v>
       </c>
       <c r="U5" s="11">
         <f t="shared" si="0"/>
-        <v>45165</v>
+        <v>45172</v>
       </c>
       <c r="V5" s="10">
         <f>U5+1</f>
-        <v>45166</v>
+        <v>45173</v>
       </c>
       <c r="W5" s="9">
         <f>V5+1</f>
-        <v>45167</v>
+        <v>45174</v>
       </c>
       <c r="X5" s="9">
         <f t="shared" si="0"/>
-        <v>45168</v>
+        <v>45175</v>
       </c>
       <c r="Y5" s="9">
         <f t="shared" si="0"/>
-        <v>45169</v>
+        <v>45176</v>
       </c>
       <c r="Z5" s="9">
         <f t="shared" si="0"/>
-        <v>45170</v>
+        <v>45177</v>
       </c>
       <c r="AA5" s="9">
         <f t="shared" si="0"/>
-        <v>45171</v>
+        <v>45178</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="0"/>
-        <v>45172</v>
+        <v>45179</v>
       </c>
       <c r="AC5" s="10">
         <f>AB5+1</f>
-        <v>45173</v>
+        <v>45180</v>
       </c>
       <c r="AD5" s="9">
         <f>AC5+1</f>
-        <v>45174</v>
+        <v>45181</v>
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="0"/>
-        <v>45175</v>
+        <v>45182</v>
       </c>
       <c r="AF5" s="9">
         <f t="shared" si="0"/>
-        <v>45176</v>
+        <v>45183</v>
       </c>
       <c r="AG5" s="9">
         <f t="shared" si="0"/>
-        <v>45177</v>
+        <v>45184</v>
       </c>
       <c r="AH5" s="9">
         <f t="shared" si="0"/>
-        <v>45178</v>
+        <v>45185</v>
       </c>
       <c r="AI5" s="11">
         <f t="shared" si="0"/>
-        <v>45179</v>
+        <v>45186</v>
       </c>
       <c r="AJ5" s="10">
         <f>AI5+1</f>
-        <v>45180</v>
+        <v>45187</v>
       </c>
       <c r="AK5" s="9">
         <f>AJ5+1</f>
-        <v>45181</v>
+        <v>45188</v>
       </c>
       <c r="AL5" s="9">
         <f t="shared" si="0"/>
-        <v>45182</v>
+        <v>45189</v>
       </c>
       <c r="AM5" s="9">
         <f t="shared" si="0"/>
-        <v>45183</v>
+        <v>45190</v>
       </c>
       <c r="AN5" s="9">
         <f t="shared" si="0"/>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="AO5" s="9">
         <f t="shared" si="0"/>
-        <v>45185</v>
+        <v>45192</v>
       </c>
       <c r="AP5" s="11">
         <f t="shared" si="0"/>
-        <v>45186</v>
+        <v>45193</v>
       </c>
       <c r="AQ5" s="10">
         <f>AP5+1</f>
-        <v>45187</v>
+        <v>45194</v>
       </c>
       <c r="AR5" s="9">
         <f>AQ5+1</f>
-        <v>45188</v>
+        <v>45195</v>
       </c>
       <c r="AS5" s="9">
         <f t="shared" si="0"/>
-        <v>45189</v>
+        <v>45196</v>
       </c>
       <c r="AT5" s="9">
         <f t="shared" si="0"/>
-        <v>45190</v>
+        <v>45197</v>
       </c>
       <c r="AU5" s="9">
         <f t="shared" si="0"/>
-        <v>45191</v>
+        <v>45198</v>
       </c>
       <c r="AV5" s="9">
         <f t="shared" si="0"/>
-        <v>45192</v>
+        <v>45199</v>
       </c>
       <c r="AW5" s="11">
         <f t="shared" si="0"/>
-        <v>45193</v>
+        <v>45200</v>
       </c>
       <c r="AX5" s="10">
         <f>AW5+1</f>
-        <v>45194</v>
+        <v>45201</v>
       </c>
       <c r="AY5" s="9">
         <f>AX5+1</f>
-        <v>45195</v>
+        <v>45202</v>
       </c>
       <c r="AZ5" s="9">
         <f t="shared" ref="AZ5:BD5" si="1">AY5+1</f>
-        <v>45196</v>
+        <v>45203</v>
       </c>
       <c r="BA5" s="9">
         <f t="shared" si="1"/>
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="BB5" s="9">
         <f t="shared" si="1"/>
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="BC5" s="9">
         <f t="shared" si="1"/>
-        <v>45199</v>
+        <v>45206</v>
       </c>
       <c r="BD5" s="11">
         <f t="shared" si="1"/>
-        <v>45200</v>
+        <v>45207</v>
       </c>
       <c r="BE5" s="10">
         <f>BD5+1</f>
-        <v>45201</v>
+        <v>45208</v>
       </c>
       <c r="BF5" s="9">
         <f>BE5+1</f>
-        <v>45202</v>
+        <v>45209</v>
       </c>
       <c r="BG5" s="9">
         <f t="shared" ref="BG5:BK5" si="2">BF5+1</f>
-        <v>45203</v>
+        <v>45210</v>
       </c>
       <c r="BH5" s="9">
         <f t="shared" si="2"/>
-        <v>45204</v>
+        <v>45211</v>
       </c>
       <c r="BI5" s="9">
         <f t="shared" si="2"/>
-        <v>45205</v>
+        <v>45212</v>
       </c>
       <c r="BJ5" s="9">
         <f t="shared" si="2"/>
-        <v>45206</v>
+        <v>45213</v>
       </c>
       <c r="BK5" s="11">
         <f t="shared" si="2"/>
-        <v>45207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
         <v>31</v>
       </c>
@@ -1793,7 +1791,7 @@
         <v>T</v>
       </c>
       <c r="J6" s="12" t="str">
-        <f t="shared" ref="I6:AQ6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AQ6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>W</v>
       </c>
       <c r="K6" s="12" t="str">
@@ -2009,7 +2007,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
         <v>36</v>
       </c>
@@ -2075,7 +2073,7 @@
       <c r="BJ7" s="34"/>
       <c r="BK7" s="34"/>
     </row>
-    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="49" t="s">
         <v>32</v>
       </c>
@@ -2147,11 +2145,11 @@
       <c r="BJ8" s="34"/>
       <c r="BK8" s="34"/>
     </row>
-    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="60" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="18">
@@ -2225,11 +2223,11 @@
       <c r="BJ9" s="34"/>
       <c r="BK9" s="34"/>
     </row>
-    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="60" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="18">
@@ -2303,9 +2301,9 @@
       <c r="BJ10" s="34"/>
       <c r="BK10" s="34"/>
     </row>
-    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="48"/>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="60" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="18">
@@ -2379,9 +2377,9 @@
       <c r="BJ11" s="34"/>
       <c r="BK11" s="34"/>
     </row>
-    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="60" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="18">
@@ -2455,9 +2453,9 @@
       <c r="BJ12" s="34"/>
       <c r="BK12" s="34"/>
     </row>
-    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="48"/>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="60" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="18"/>
@@ -2529,7 +2527,7 @@
       <c r="BJ13" s="34"/>
       <c r="BK13" s="34"/>
     </row>
-    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="49" t="s">
         <v>34</v>
       </c>
@@ -2601,24 +2599,24 @@
       <c r="BJ14" s="34"/>
       <c r="BK14" s="34"/>
     </row>
-    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49"/>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="61" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="23">
         <v>0.5</v>
       </c>
       <c r="D15" s="21">
-        <v>45179</v>
+        <v>45194</v>
       </c>
       <c r="E15" s="21">
-        <v>45189</v>
+        <v>45198</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -2677,24 +2675,24 @@
       <c r="BJ15" s="34"/>
       <c r="BK15" s="34"/>
     </row>
-    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="48"/>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="61" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="23">
         <v>0.5</v>
       </c>
       <c r="D16" s="21">
-        <v>45189</v>
+        <v>45194</v>
       </c>
       <c r="E16" s="21">
-        <v>45194</v>
+        <v>45198</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
@@ -2753,22 +2751,22 @@
       <c r="BJ16" s="34"/>
       <c r="BK16" s="34"/>
     </row>
-    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="48"/>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="61" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="21">
-        <v>45194</v>
+        <v>45195</v>
       </c>
       <c r="E17" s="21">
-        <v>45196</v>
+        <v>45199</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -2827,22 +2825,22 @@
       <c r="BJ17" s="34"/>
       <c r="BK17" s="34"/>
     </row>
-    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="61" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="21">
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="E18" s="21">
-        <v>45197</v>
+        <v>45200</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
@@ -2901,22 +2899,22 @@
       <c r="BJ18" s="34"/>
       <c r="BK18" s="34"/>
     </row>
-    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="48"/>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="61" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="21">
-        <v>45197</v>
+        <v>45200</v>
       </c>
       <c r="E19" s="21">
-        <v>45197</v>
+        <v>45206</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -2975,7 +2973,7 @@
       <c r="BJ19" s="34"/>
       <c r="BK19" s="34"/>
     </row>
-    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="48" t="s">
         <v>25</v>
       </c>
@@ -3047,17 +3045,17 @@
       <c r="BJ20" s="34"/>
       <c r="BK20" s="34"/>
     </row>
-    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="48"/>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="62" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="26">
-        <v>45197</v>
+        <v>45204</v>
       </c>
       <c r="E21" s="26">
-        <v>45200</v>
+        <v>45207</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14">
@@ -3121,9 +3119,9 @@
       <c r="BJ21" s="34"/>
       <c r="BK21" s="34"/>
     </row>
-    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="48"/>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="62" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="28"/>
@@ -3131,12 +3129,12 @@
         <v>45200</v>
       </c>
       <c r="E22" s="26">
-        <v>45201</v>
+        <v>45206</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
@@ -3195,22 +3193,22 @@
       <c r="BJ22" s="34"/>
       <c r="BK22" s="34"/>
     </row>
-    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="48"/>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="62" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="26">
-        <v>45201</v>
+        <v>45200</v>
       </c>
       <c r="E23" s="26">
-        <v>45204</v>
+        <v>45205</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -3269,9 +3267,9 @@
       <c r="BJ23" s="34"/>
       <c r="BK23" s="34"/>
     </row>
-    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="48"/>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="62" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="28"/>
@@ -3343,9 +3341,9 @@
       <c r="BJ24" s="34"/>
       <c r="BK24" s="34"/>
     </row>
-    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="48"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="62" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="28"/>
@@ -3417,7 +3415,7 @@
       <c r="BJ25" s="34"/>
       <c r="BK25" s="34"/>
     </row>
-    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="48" t="s">
         <v>27</v>
       </c>
@@ -3487,7 +3485,7 @@
       <c r="BJ26" s="34"/>
       <c r="BK26" s="34"/>
     </row>
-    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="49" t="s">
         <v>26</v>
       </c>
@@ -3559,10 +3557,10 @@
       <c r="BJ27" s="36"/>
       <c r="BK27" s="36"/>
     </row>
-    <row r="28" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E29" s="50"/>
     </row>
   </sheetData>
@@ -3633,7 +3631,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="D4">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -3698,101 +3696,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="38" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="87.109375" style="38" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="40" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="39"/>
     </row>
-    <row r="3" spans="1:2" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="44" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="45"/>
     </row>
-    <row r="4" spans="1:2" s="41" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="38" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="38" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="41" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="42" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="38" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="38" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="41" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="42" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="38" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="38" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="41" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" s="41" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>